<commit_message>
Updated the model to fix leakage and now use xgboost
</commit_message>
<xml_diff>
--- a/prediction_tracker.xlsx
+++ b/prediction_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nboys\College Basketball Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F70719-B2DC-40A3-AA03-F3F6EB16AEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C9095B-80E9-4CED-BD51-925CF1D94AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="505">
   <si>
     <t>prediction_date</t>
   </si>
@@ -1465,10 +1465,49 @@
     <t>CONSIDER High Point -24.5</t>
   </si>
   <si>
+    <t>home_games_played</t>
+  </si>
+  <si>
+    <t>away_games_played</t>
+  </si>
+  <si>
     <t>2025-11-18</t>
   </si>
   <si>
-    <t>BET Buffalo +2.5</t>
+    <t>BET American +14.5</t>
+  </si>
+  <si>
+    <t>BET Michigan St. +4.5</t>
+  </si>
+  <si>
+    <t>BET Hampton +11.5</t>
+  </si>
+  <si>
+    <t>BET Drexel -12.5</t>
+  </si>
+  <si>
+    <t>BET Princeton +3.5</t>
+  </si>
+  <si>
+    <t>BET Radford +9.5</t>
+  </si>
+  <si>
+    <t>BET Little Rock +14.5</t>
+  </si>
+  <si>
+    <t>BET Purdue Fort Wayne +12.5</t>
+  </si>
+  <si>
+    <t>BET Evansville -2.5</t>
+  </si>
+  <si>
+    <t>BET Boise St. -9.5</t>
+  </si>
+  <si>
+    <t>BET Kansas +11.5</t>
+  </si>
+  <si>
+    <t>BET Nevada -12.5</t>
   </si>
   <si>
     <t>North Carolina A&amp;T</t>
@@ -1477,130 +1516,34 @@
     <t>BET Morgan St. +2.5</t>
   </si>
   <si>
-    <t>BET Evansville -2.5</t>
-  </si>
-  <si>
     <t>Pepperdine</t>
   </si>
   <si>
     <t>BET Pepperdine -4.5</t>
   </si>
   <si>
-    <t>BET Iona -3.5</t>
-  </si>
-  <si>
-    <t>BET James Madison +2.5</t>
-  </si>
-  <si>
-    <t>BET Yale -8.5</t>
-  </si>
-  <si>
-    <t>BET Kentucky -4.5</t>
+    <t>BET Grambling St. +6.5</t>
+  </si>
+  <si>
+    <t>BET Rhode Island +8.5</t>
+  </si>
+  <si>
+    <t>BET Holy Cross +3.5</t>
+  </si>
+  <si>
+    <t>BET Towson -2.5</t>
+  </si>
+  <si>
+    <t>BET Xavier -10.5</t>
+  </si>
+  <si>
+    <t>BET Buffalo +3.5</t>
   </si>
   <si>
     <t>East Carolina</t>
   </si>
   <si>
-    <t>BET UNC Wilmington -5.5</t>
-  </si>
-  <si>
-    <t>BET Brown -3.5</t>
-  </si>
-  <si>
-    <t>BET Drexel -12.5</t>
-  </si>
-  <si>
-    <t>BET Boise St. -9.5</t>
-  </si>
-  <si>
-    <t>BET San Diego -6.5</t>
-  </si>
-  <si>
-    <t>BET South Carolina -9.5</t>
-  </si>
-  <si>
-    <t>BET Utah -12.5</t>
-  </si>
-  <si>
-    <t>BET Columbia -6.5</t>
-  </si>
-  <si>
-    <t>BET Texas A&amp;M -17.5</t>
-  </si>
-  <si>
-    <t>BET Murray St. -14.5</t>
-  </si>
-  <si>
-    <t>BET George Mason -15.5</t>
-  </si>
-  <si>
-    <t>LEAN Duke -11.5</t>
-  </si>
-  <si>
-    <t>LEAN Boston College -11.5</t>
-  </si>
-  <si>
-    <t>LEAN Xavier -10.5</t>
-  </si>
-  <si>
-    <t>LEAN Arkansas -22.5</t>
-  </si>
-  <si>
-    <t>San Diego St.</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>LEAN San Diego St. -15.5</t>
-  </si>
-  <si>
-    <t>LEAN Nevada -12.5</t>
-  </si>
-  <si>
-    <t>Rider</t>
-  </si>
-  <si>
-    <t>LEAN Rider +30.5</t>
-  </si>
-  <si>
-    <t>LEAN Rutgers -14.5</t>
-  </si>
-  <si>
-    <t>LEAN Mississippi -22.5</t>
-  </si>
-  <si>
-    <t>CONSIDER San Francisco -19.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Alcorn St. +32.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Syracuse -21.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Florida St. -20.5</t>
-  </si>
-  <si>
-    <t>CONSIDER North Carolina -25.5</t>
-  </si>
-  <si>
-    <t>CONSIDER DePaul -22.5</t>
-  </si>
-  <si>
-    <t>CONSIDER UCLA -28.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Cornell -17.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Stanford -20.5</t>
-  </si>
-  <si>
-    <t>CONSIDER Seton Hall -25.5</t>
-  </si>
-  <si>
-    <t>CONSIDER California -22.5</t>
+    <t>LEAN UNC Wilmington -6.5</t>
   </si>
 </sst>
 </file>
@@ -2793,23 +2736,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1015625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2846,118 +2784,142 @@
       <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M1" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>-14.5</v>
       </c>
       <c r="E2">
-        <v>0.91052057363190442</v>
+        <v>2.3181600841518009E-19</v>
       </c>
       <c r="F2" t="s">
         <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="J2">
-        <v>-4.4075517817605743</v>
+        <v>7.9315647472664486</v>
       </c>
       <c r="K2">
-        <v>4.6019669841059709</v>
+        <v>-9.0546504971375583</v>
       </c>
       <c r="L2">
-        <v>-0.20259940515951319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.4282889880974679</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>480</v>
+        <v>286</v>
       </c>
       <c r="D3">
-        <v>2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="E3">
-        <v>0.90509992153478824</v>
+        <v>4.3611671311540685E-22</v>
       </c>
       <c r="F3" t="s">
         <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="J3">
-        <v>-1.1499258298008641</v>
+        <v>4.0942531661255259</v>
       </c>
       <c r="K3">
-        <v>2.7237361760804788</v>
+        <v>0.52651588834319796</v>
       </c>
       <c r="L3">
-        <v>-5.5498223692212897E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.6989590068516402E-2</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>398</v>
       </c>
       <c r="C4" t="s">
-        <v>376</v>
+        <v>112</v>
       </c>
       <c r="D4">
-        <v>-2.5</v>
+        <v>-11.5</v>
       </c>
       <c r="E4">
-        <v>0.89999364766285861</v>
+        <v>1.9831397683253601E-20</v>
       </c>
       <c r="F4" t="s">
         <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="J4">
-        <v>-1.298775610906759</v>
+        <v>5.2697196560410617</v>
       </c>
       <c r="K4">
-        <v>1.0683888404247599</v>
+        <v>-5.2098069384111483</v>
       </c>
       <c r="L4">
-        <v>-6.1445319984146603E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.2759028038949457</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B5" t="s">
-        <v>483</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>373</v>
       </c>
       <c r="D5">
-        <v>-4.5</v>
+        <v>-12.5</v>
       </c>
       <c r="E5">
-        <v>0.89076143934359597</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>89</v>
@@ -2966,18 +2928,24 @@
         <v>484</v>
       </c>
       <c r="J5">
-        <v>-5.0958382562571529</v>
+        <v>2.0051418511613832</v>
       </c>
       <c r="K5">
-        <v>-1.8079227748023361</v>
+        <v>-2.8776287062775618</v>
       </c>
       <c r="L5">
-        <v>-8.0966371877400606E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>9.6900302184999898E-2</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B6" t="s">
         <v>344</v>
@@ -2989,7 +2957,7 @@
         <v>-3.5</v>
       </c>
       <c r="E6">
-        <v>0.887439030670234</v>
+        <v>3.353133508549073E-31</v>
       </c>
       <c r="F6" t="s">
         <v>89</v>
@@ -3006,22 +2974,28 @@
       <c r="L6">
         <v>8.2270441129082605E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s">
-        <v>348</v>
+        <v>130</v>
       </c>
       <c r="D7">
-        <v>2.5</v>
+        <v>-9.5</v>
       </c>
       <c r="E7">
-        <v>0.88673646582780319</v>
+        <v>1.978452512143979E-19</v>
       </c>
       <c r="F7" t="s">
         <v>89</v>
@@ -3030,30 +3004,36 @@
         <v>486</v>
       </c>
       <c r="J7">
-        <v>3.1576968835152002</v>
+        <v>1.1980208288685641</v>
       </c>
       <c r="K7">
-        <v>5.9159255307837668</v>
+        <v>-5.8662816115774916</v>
       </c>
       <c r="L7">
-        <v>-7.5077113943064294E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1836121916601304</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>221</v>
       </c>
       <c r="D8">
-        <v>-8.5</v>
+        <v>-14.5</v>
       </c>
       <c r="E8">
-        <v>0.86791033018940644</v>
+        <v>1.235146570842163E-33</v>
       </c>
       <c r="F8" t="s">
         <v>89</v>
@@ -3062,30 +3042,36 @@
         <v>487</v>
       </c>
       <c r="J8">
-        <v>7.7179329851954179</v>
+        <v>3.8237311730329822</v>
       </c>
       <c r="K8">
-        <v>-1.7571199542921361</v>
+        <v>-1.783492398574438</v>
       </c>
       <c r="L8">
-        <v>0.22703274848116911</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.14795479375997819</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="D9">
-        <v>-4.5</v>
+        <v>-12.5</v>
       </c>
       <c r="E9">
-        <v>0.86662422386799698</v>
+        <v>4.0193966184714482E-20</v>
       </c>
       <c r="F9" t="s">
         <v>89</v>
@@ -3094,158 +3080,188 @@
         <v>488</v>
       </c>
       <c r="J9">
-        <v>4.0942531661255259</v>
+        <v>8.972146988766923</v>
       </c>
       <c r="K9">
-        <v>0.52651588834319796</v>
+        <v>-3.9217690961916531</v>
       </c>
       <c r="L9">
-        <v>2.6989590068516402E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.33006252418946908</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B10" t="s">
-        <v>418</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
-        <v>489</v>
+        <v>376</v>
       </c>
       <c r="D10">
-        <v>-5.5</v>
+        <v>-2.5</v>
       </c>
       <c r="E10">
-        <v>0.85926533827602236</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="F10" t="s">
         <v>89</v>
       </c>
       <c r="G10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J10">
-        <v>2.4635388029266641</v>
+        <v>-1.298775610906759</v>
       </c>
       <c r="K10">
-        <v>-0.37759259856051131</v>
+        <v>1.0683888404247599</v>
       </c>
       <c r="L10">
-        <v>7.5823938067789795E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>-6.1445319984146603E-2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>422</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>306</v>
       </c>
       <c r="D11">
-        <v>-3.5</v>
+        <v>-9.5</v>
       </c>
       <c r="E11">
-        <v>0.85188148375631156</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="F11" t="s">
         <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J11">
-        <v>-2.3455234356986669</v>
+        <v>3.7882683522767309</v>
       </c>
       <c r="K11">
-        <v>-7.9470341170601841</v>
+        <v>-4.9625599646535079</v>
       </c>
       <c r="L11">
-        <v>0.1080583170330956</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1759108193672016</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>373</v>
+        <v>101</v>
       </c>
       <c r="D12">
-        <v>-12.5</v>
+        <v>-11.5</v>
       </c>
       <c r="E12">
-        <v>0.84387121131779186</v>
+        <v>8.270497318391176E-14</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
       </c>
       <c r="G12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J12">
-        <v>2.0051418511613832</v>
+        <v>5.1655830789215136</v>
       </c>
       <c r="K12">
-        <v>-2.8776287062775618</v>
+        <v>-0.89885998176538351</v>
       </c>
       <c r="L12">
-        <v>9.6900302184999898E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>3.8136087875158403E-2</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B13" t="s">
-        <v>422</v>
+        <v>279</v>
       </c>
       <c r="C13" t="s">
-        <v>306</v>
+        <v>53</v>
       </c>
       <c r="D13">
-        <v>-9.5</v>
+        <v>-12.5</v>
       </c>
       <c r="E13">
-        <v>0.83078338752897007</v>
+        <v>0.99999999999987743</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" t="s">
+        <v>492</v>
+      </c>
+      <c r="J13">
+        <v>6.2520870894462064</v>
+      </c>
+      <c r="K13">
+        <v>-1.626292581933882</v>
+      </c>
+      <c r="L13">
+        <v>0.21253096752498221</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>480</v>
+      </c>
+      <c r="B14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" t="s">
         <v>493</v>
       </c>
-      <c r="J13">
-        <v>3.7882683522767309</v>
-      </c>
-      <c r="K13">
-        <v>-4.9625599646535079</v>
-      </c>
-      <c r="L13">
-        <v>0.1759108193672016</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>478</v>
-      </c>
-      <c r="B14" t="s">
-        <v>204</v>
-      </c>
-      <c r="C14" t="s">
-        <v>292</v>
-      </c>
       <c r="D14">
-        <v>-6.5</v>
+        <v>2.5</v>
       </c>
       <c r="E14">
-        <v>0.80039792669931742</v>
+        <v>0.99999999999976152</v>
       </c>
       <c r="F14" t="s">
         <v>89</v>
@@ -3254,845 +3270,323 @@
         <v>494</v>
       </c>
       <c r="J14">
-        <v>8.0326170766720821</v>
+        <v>-1.1499258298008641</v>
       </c>
       <c r="K14">
-        <v>-8.3630683208582399E-2</v>
+        <v>2.7237361760804788</v>
       </c>
       <c r="L14">
-        <v>0.20184719283795879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>-5.5498223692212897E-2</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>495</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="D15">
-        <v>-9.5</v>
+        <v>-4.5</v>
       </c>
       <c r="E15">
-        <v>0.79498724542047827</v>
+        <v>0.99999999999967071</v>
       </c>
       <c r="F15" t="s">
         <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="J15">
-        <v>1.1980208288685641</v>
+        <v>-5.0958382562571529</v>
       </c>
       <c r="K15">
-        <v>-5.8662816115774916</v>
+        <v>-1.8079227748023361</v>
       </c>
       <c r="L15">
-        <v>0.1836121916601304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>-8.0966371877400606E-2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>292</v>
       </c>
       <c r="D16">
-        <v>-12.5</v>
+        <v>-6.5</v>
       </c>
       <c r="E16">
-        <v>0.78824208260717243</v>
+        <v>1.3916211993561761E-11</v>
       </c>
       <c r="F16" t="s">
         <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J16">
-        <v>8.972146988766923</v>
+        <v>8.0326170766720821</v>
       </c>
       <c r="K16">
-        <v>-3.9217690961916531</v>
+        <v>-8.3630683208582399E-2</v>
       </c>
       <c r="L16">
-        <v>0.33006252418946908</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.20184719283795879</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
+        <v>119</v>
       </c>
       <c r="D17">
-        <v>-6.5</v>
+        <v>-8.5</v>
       </c>
       <c r="E17">
-        <v>0.78732246303732134</v>
+        <v>1.4783733368527839E-11</v>
       </c>
       <c r="F17" t="s">
         <v>89</v>
       </c>
       <c r="G17" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="J17">
-        <v>3.4942780800506001E-2</v>
+        <v>7.7179329851954179</v>
       </c>
       <c r="K17">
-        <v>-1.679010114857292</v>
+        <v>-1.7571199542921361</v>
       </c>
       <c r="L17">
-        <v>3.9260916599151298E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.22703274848116911</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="D18">
-        <v>-17.5</v>
+        <v>-3.5</v>
       </c>
       <c r="E18">
-        <v>0.7725992568273885</v>
+        <v>7.2083830541785769E-9</v>
       </c>
       <c r="F18" t="s">
         <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="J18">
-        <v>8.4200485270847878</v>
+        <v>-2.3455234356986669</v>
       </c>
       <c r="K18">
-        <v>-8.214669305578596</v>
+        <v>-7.9470341170601841</v>
       </c>
       <c r="L18">
-        <v>0.37562196554244442</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1080583170330956</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>221</v>
+        <v>348</v>
       </c>
       <c r="D19">
-        <v>-14.5</v>
+        <v>2.5</v>
       </c>
       <c r="E19">
-        <v>0.7650701537546164</v>
+        <v>2.5456972609238969E-7</v>
       </c>
       <c r="F19" t="s">
         <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="J19">
-        <v>3.8237311730329822</v>
+        <v>3.1576968835152002</v>
       </c>
       <c r="K19">
-        <v>-1.783492398574438</v>
+        <v>5.9159255307837668</v>
       </c>
       <c r="L19">
-        <v>0.14795479375997819</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>-7.5077113943064294E-2</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B20" t="s">
-        <v>435</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="D20">
-        <v>-15.5</v>
+        <v>-10.5</v>
       </c>
       <c r="E20">
-        <v>0.75136520684177555</v>
+        <v>0.99990245974823644</v>
       </c>
       <c r="F20" t="s">
         <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="J20">
-        <v>5.5991874818179639</v>
+        <v>1.5245152028601301</v>
       </c>
       <c r="K20">
-        <v>-7.2598325518603133</v>
+        <v>-8.3663363222176201</v>
       </c>
       <c r="L20">
-        <v>0.33959647129934961</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.2599889565876975</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="D21">
-        <v>-11.5</v>
+        <v>3.5</v>
       </c>
       <c r="E21">
-        <v>0.73900292230220177</v>
+        <v>0.99835493914236317</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="G21" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="J21">
-        <v>5.1655830789215136</v>
+        <v>-4.4075517817605743</v>
       </c>
       <c r="K21">
-        <v>-0.89885998176538351</v>
+        <v>4.6019669841059709</v>
       </c>
       <c r="L21">
-        <v>3.8136087875158403E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>-0.20259940515951319</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B22" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>503</v>
       </c>
       <c r="D22">
-        <v>-11.5</v>
+        <v>-6.5</v>
       </c>
       <c r="E22">
-        <v>0.72412135044461678</v>
+        <v>0.79551547598932848</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="J22">
-        <v>5.2697196560410617</v>
+        <v>2.4635388029266641</v>
       </c>
       <c r="K22">
-        <v>-5.2098069384111483</v>
+        <v>-0.37759259856051131</v>
       </c>
       <c r="L22">
-        <v>0.2759028038949457</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>478</v>
-      </c>
-      <c r="B23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23">
-        <v>-10.5</v>
-      </c>
-      <c r="E23">
-        <v>0.71148768973128917</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>503</v>
-      </c>
-      <c r="J23">
-        <v>1.5245152028601301</v>
-      </c>
-      <c r="K23">
-        <v>-8.3663363222176201</v>
-      </c>
-      <c r="L23">
-        <v>0.2599889565876975</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>478</v>
-      </c>
-      <c r="B24" t="s">
-        <v>359</v>
-      </c>
-      <c r="C24" t="s">
-        <v>370</v>
-      </c>
-      <c r="D24">
-        <v>-22.5</v>
-      </c>
-      <c r="E24">
-        <v>0.70449719282397605</v>
-      </c>
-      <c r="F24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" t="s">
-        <v>504</v>
-      </c>
-      <c r="J24">
-        <v>12.5528839141988</v>
-      </c>
-      <c r="K24">
-        <v>-9.9308735088086024</v>
-      </c>
-      <c r="L24">
-        <v>0.44772343842787371</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>478</v>
-      </c>
-      <c r="B25" t="s">
-        <v>505</v>
-      </c>
-      <c r="C25" t="s">
-        <v>506</v>
-      </c>
-      <c r="D25">
-        <v>-15.5</v>
-      </c>
-      <c r="E25">
-        <v>0.69289542379006708</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" t="s">
-        <v>507</v>
-      </c>
-      <c r="J25">
-        <v>4.3911058431210392</v>
-      </c>
-      <c r="K25">
-        <v>-7.8896410878533354</v>
-      </c>
-      <c r="L25">
-        <v>0.2656711904803773</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>478</v>
-      </c>
-      <c r="B26" t="s">
-        <v>279</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26">
-        <v>-12.5</v>
-      </c>
-      <c r="E26">
-        <v>0.69187484046467462</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" t="s">
-        <v>508</v>
-      </c>
-      <c r="J26">
-        <v>6.2520870894462064</v>
-      </c>
-      <c r="K26">
-        <v>-1.626292581933882</v>
-      </c>
-      <c r="L26">
-        <v>0.21253096752498221</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>478</v>
-      </c>
-      <c r="B27" t="s">
-        <v>207</v>
-      </c>
-      <c r="C27" t="s">
-        <v>509</v>
-      </c>
-      <c r="D27">
-        <v>-30.5</v>
-      </c>
-      <c r="E27">
-        <v>0.32003431956343958</v>
-      </c>
-      <c r="F27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" t="s">
-        <v>510</v>
-      </c>
-      <c r="J27">
-        <v>15.644465285876359</v>
-      </c>
-      <c r="K27">
-        <v>-13.56613651632132</v>
-      </c>
-      <c r="L27">
-        <v>0.64913809062549832</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>478</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" t="s">
-        <v>274</v>
-      </c>
-      <c r="D28">
-        <v>-14.5</v>
-      </c>
-      <c r="E28">
-        <v>0.67968942602399041</v>
-      </c>
-      <c r="F28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" t="s">
-        <v>511</v>
-      </c>
-      <c r="J28">
-        <v>7.9315647472664486</v>
-      </c>
-      <c r="K28">
-        <v>-9.0546504971375583</v>
-      </c>
-      <c r="L28">
-        <v>0.4282889880974679</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>478</v>
-      </c>
-      <c r="B29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29">
-        <v>-22.5</v>
-      </c>
-      <c r="E29">
-        <v>0.66813649922484941</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" t="s">
-        <v>512</v>
-      </c>
-      <c r="J29">
-        <v>14.769953749765479</v>
-      </c>
-      <c r="K29">
-        <v>-5.8819039043259522</v>
-      </c>
-      <c r="L29">
-        <v>0.47008322189184337</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>478</v>
-      </c>
-      <c r="B30" t="s">
-        <v>269</v>
-      </c>
-      <c r="C30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30">
-        <v>-19.5</v>
-      </c>
-      <c r="E30">
-        <v>0.64150773737754618</v>
-      </c>
-      <c r="F30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" t="s">
-        <v>513</v>
-      </c>
-      <c r="J30">
-        <v>8.3167837107190223</v>
-      </c>
-      <c r="K30">
-        <v>-10.844677352214401</v>
-      </c>
-      <c r="L30">
-        <v>0.46896981700920609</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>478</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31">
-        <v>-32.5</v>
-      </c>
-      <c r="E31">
-        <v>0.38434216940956911</v>
-      </c>
-      <c r="F31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" t="s">
-        <v>514</v>
-      </c>
-      <c r="J31">
-        <v>16.447843824640572</v>
-      </c>
-      <c r="K31">
-        <v>-11.578074277557381</v>
-      </c>
-      <c r="L31">
-        <v>0.63391732064858686</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>478</v>
-      </c>
-      <c r="B32" t="s">
-        <v>434</v>
-      </c>
-      <c r="C32" t="s">
-        <v>300</v>
-      </c>
-      <c r="D32">
-        <v>-21.5</v>
-      </c>
-      <c r="E32">
-        <v>0.61322504557565849</v>
-      </c>
-      <c r="F32" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" t="s">
-        <v>515</v>
-      </c>
-      <c r="J32">
-        <v>11.84132880181096</v>
-      </c>
-      <c r="K32">
-        <v>-6.7430776177236709</v>
-      </c>
-      <c r="L32">
-        <v>0.43060395330859708</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>478</v>
-      </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>264</v>
-      </c>
-      <c r="D33">
-        <v>-20.5</v>
-      </c>
-      <c r="E33">
-        <v>0.60385342410485432</v>
-      </c>
-      <c r="F33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" t="s">
-        <v>516</v>
-      </c>
-      <c r="J33">
-        <v>12.24541382037201</v>
-      </c>
-      <c r="K33">
-        <v>-10.16852344719277</v>
-      </c>
-      <c r="L33">
-        <v>0.5419322875744168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>478</v>
-      </c>
-      <c r="B34" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34">
-        <v>-25.5</v>
-      </c>
-      <c r="E34">
-        <v>0.59635841989206406</v>
-      </c>
-      <c r="F34" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" t="s">
-        <v>517</v>
-      </c>
-      <c r="J34">
-        <v>11.945484362619201</v>
-      </c>
-      <c r="K34">
-        <v>-12.50113898027173</v>
-      </c>
-      <c r="L34">
-        <v>0.49137414176276578</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>478</v>
-      </c>
-      <c r="B35" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" t="s">
-        <v>414</v>
-      </c>
-      <c r="D35">
-        <v>-22.5</v>
-      </c>
-      <c r="E35">
-        <v>0.59088918675223212</v>
-      </c>
-      <c r="F35" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" t="s">
-        <v>518</v>
-      </c>
-      <c r="J35">
-        <v>14.131018386137169</v>
-      </c>
-      <c r="K35">
-        <v>-10.15375140127901</v>
-      </c>
-      <c r="L35">
-        <v>0.55983878389195341</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>478</v>
-      </c>
-      <c r="B36" t="s">
-        <v>328</v>
-      </c>
-      <c r="C36" t="s">
-        <v>334</v>
-      </c>
-      <c r="D36">
-        <v>-28.5</v>
-      </c>
-      <c r="E36">
-        <v>0.58630689192962782</v>
-      </c>
-      <c r="F36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" t="s">
-        <v>519</v>
-      </c>
-      <c r="J36">
-        <v>13.36470540473276</v>
-      </c>
-      <c r="K36">
-        <v>-15.497531640913831</v>
-      </c>
-      <c r="L36">
-        <v>0.59566289497632474</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>478</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37">
-        <v>-17.5</v>
-      </c>
-      <c r="E37">
-        <v>0.57482864855894888</v>
-      </c>
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" t="s">
-        <v>520</v>
-      </c>
-      <c r="J37">
-        <v>12.012877917112601</v>
-      </c>
-      <c r="K37">
-        <v>-4.0280044171164064</v>
-      </c>
-      <c r="L37">
-        <v>0.32184991301177851</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>478</v>
-      </c>
-      <c r="B38" t="s">
-        <v>260</v>
-      </c>
-      <c r="C38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D38">
-        <v>-20.5</v>
-      </c>
-      <c r="E38">
-        <v>0.56937924156741837</v>
-      </c>
-      <c r="F38" t="s">
-        <v>36</v>
-      </c>
-      <c r="G38" t="s">
-        <v>521</v>
-      </c>
-      <c r="J38">
-        <v>4.3796118086438156</v>
-      </c>
-      <c r="K38">
-        <v>-9.1138649187133183</v>
-      </c>
-      <c r="L38">
-        <v>0.34904845067183138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>478</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>380</v>
-      </c>
-      <c r="D39">
-        <v>-25.5</v>
-      </c>
-      <c r="E39">
-        <v>0.5627086213127428</v>
-      </c>
-      <c r="F39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" t="s">
-        <v>522</v>
-      </c>
-      <c r="J39">
-        <v>13.982709928513261</v>
-      </c>
-      <c r="K39">
-        <v>-8.6502333671711966</v>
-      </c>
-      <c r="L39">
-        <v>0.51733732989642811</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>478</v>
-      </c>
-      <c r="B40" t="s">
-        <v>305</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40">
-        <v>-22.5</v>
-      </c>
-      <c r="E40">
-        <v>0.56131792855328289</v>
-      </c>
-      <c r="F40" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" t="s">
-        <v>523</v>
-      </c>
-      <c r="J40">
-        <v>10.9833621907904</v>
-      </c>
-      <c r="K40">
-        <v>-5.9119574533641384</v>
-      </c>
-      <c r="L40">
-        <v>0.42422644668279691</v>
+        <v>7.5823938067789795E-2</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>